<commit_message>
Update project xls and put all bmmls into 01_design/mockup/
</commit_message>
<xml_diff>
--- a/doc/01_design/project.xlsx
+++ b/doc/01_design/project.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="520" windowWidth="28720" windowHeight="20760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="8780" yWindow="520" windowWidth="28720" windowHeight="20760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="封面" sheetId="1" r:id="rId1"/>
     <sheet name="系统简介" sheetId="3" r:id="rId2"/>
     <sheet name="功能简介" sheetId="2" r:id="rId3"/>
     <sheet name="系统原型" sheetId="4" r:id="rId4"/>
+    <sheet name="系统架构" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>SCW管理系统企划书</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,15 +74,135 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>系统功能简介</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>系统简介</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">        本系统为问题照片整改系统。数个区可以和管理员做提交审核业务。管理员可以给区上传待整改照片，每个区也可以将整改完的照片交给管理员审核，管理员再对待审核的照片做出反馈 - 审批通过或者打回。如若打回，则区账号还可以重新修改打回的照片再次提交审核，直到通过为止。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能简介</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统原型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区账号登录界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个区的工作人员可以通过此界面登录系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 填入用户名密码登录系统。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 显示电话，审核时间，系统介绍等信息。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 可以通过联系我们功能来联系系统管理员。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区账主界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看该区有哪些待审核的问题照片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.上传整改后的照片等待审核。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 查看待整改问题照片和被打回的照片。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看该区曾近有哪些问题照片被成功审批通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区账通过审核的问题列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  查看历史审批通过条目。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区账修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果觉得账号密码不安全不好记，可以修改为更合适的密码。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  修改当前账号密码。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员主界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员通过通过审核列表来进行直观审核</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.  管理员可以给每个条目设置标记：通过、打回、关闭。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.  管理员可以给指定区上传问题照片。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员查看操作日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员可以查看所有管理员在近期的所有操作日志。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  搜索栏可以设置合适的条件范围进行筛选。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.  查看操作日志。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级管理员管理列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级管理员有权新建和禁用管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  新建和禁用当前有效管理员。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级管理员修改密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统架构</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -266,7 +387,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,8 +437,70 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -348,31 +531,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -408,8 +567,11 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="111">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -434,6 +596,37 @@
     <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -458,11 +651,389 @@
     <cellStyle name="访问过的超链接" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>234461</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10394</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>699477</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>68386</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2149230" y="4162317"/>
+          <a:ext cx="10038862" cy="7697530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>270528</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>69993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>713155</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>19535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2185297" y="14186531"/>
+          <a:ext cx="10016473" cy="8087312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>273537</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>164989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>801077</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>9768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2188306" y="23747912"/>
+          <a:ext cx="10101386" cy="8979010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>283311</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>97692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>820617</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>117229</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2198080" y="34641692"/>
+          <a:ext cx="10111152" cy="8987691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293075</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>127599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>722923</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>136766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2207844" y="45798753"/>
+          <a:ext cx="10003694" cy="6984398"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293077</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>104693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>644769</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>48845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2207846" y="54577924"/>
+          <a:ext cx="9925538" cy="7251536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>332156</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>124829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>674078</xdr:colOff>
+      <xdr:row>422</xdr:row>
+      <xdr:rowOff>136769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2246925" y="63400137"/>
+          <a:ext cx="9915768" cy="8814017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>322384</xdr:colOff>
+      <xdr:row>434</xdr:row>
+      <xdr:rowOff>61584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>654539</xdr:colOff>
+      <xdr:row>477</xdr:row>
+      <xdr:rowOff>146539</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2237153" y="74131892"/>
+          <a:ext cx="9906001" cy="7226262"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>360237</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>120484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>674076</xdr:colOff>
+      <xdr:row>541</xdr:row>
+      <xdr:rowOff>107460</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2275006" y="83158946"/>
+          <a:ext cx="9887685" cy="8789053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -789,9 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1143,51 +1712,51 @@
       <c r="N30" s="11"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="14"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="17"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="20"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1208,128 +1777,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="3:9">
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="3:9">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="3:9">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="3:9">
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="9" spans="3:9" ht="13" customHeight="1">
+      <c r="E9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="3:9">
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="3:9">
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="3:9">
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-    </row>
-    <row r="9" spans="3:9">
-      <c r="E9" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="3:9">
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="3:9">
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="3:9">
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="3:9">
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="3:9" ht="15">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="3:9" ht="13" customHeight="1">
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="3:9" ht="13" customHeight="1">
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="3:9" ht="13" customHeight="1">
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="3:9" ht="13" customHeight="1">
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="3:9" ht="15" customHeight="1">
       <c r="C14" s="3"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="3:9">
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="3:9">
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="5:9">
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="5:9">
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="5:9">
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="5:9">
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="3:9" ht="13" customHeight="1">
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="3:9" ht="13" customHeight="1">
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="5:9" ht="13" customHeight="1">
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="5:9" ht="13" customHeight="1">
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="5:9" ht="13" customHeight="1">
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="5:9" ht="13" customHeight="1">
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1338,6 +1905,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1348,197 +1916,195 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I21"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:9">
-      <c r="E2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="30" t="s">
+    <row r="2" spans="1:9" ht="19">
+      <c r="E2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="19">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" ht="19">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" ht="19">
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="30" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="30" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="31" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="31" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="31" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="31" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="31" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="32" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="32" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="32" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1557,14 +2123,331 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:I488"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="E2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B129" s="24"/>
+      <c r="C129" s="24"/>
+      <c r="D129" s="24"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" s="24"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="24"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B193" s="24"/>
+      <c r="C193" s="24"/>
+      <c r="D193" s="24"/>
+      <c r="E193" s="24"/>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B194" s="24"/>
+      <c r="C194" s="24"/>
+      <c r="D194" s="24"/>
+      <c r="E194" s="24"/>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B259" s="24"/>
+      <c r="C259" s="24"/>
+      <c r="D259" s="24"/>
+      <c r="E259" s="24"/>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B260" s="24"/>
+      <c r="C260" s="24"/>
+      <c r="D260" s="24"/>
+      <c r="E260" s="24"/>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5">
+      <c r="A313" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B313" s="24"/>
+      <c r="C313" s="24"/>
+      <c r="D313" s="24"/>
+      <c r="E313" s="24"/>
+    </row>
+    <row r="314" spans="1:5">
+      <c r="A314" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B314" s="24"/>
+      <c r="C314" s="24"/>
+      <c r="D314" s="24"/>
+      <c r="E314" s="24"/>
+    </row>
+    <row r="315" spans="1:5">
+      <c r="A315" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5">
+      <c r="A316" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5">
+      <c r="A367" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B367" s="24"/>
+      <c r="C367" s="24"/>
+      <c r="D367" s="24"/>
+      <c r="E367" s="24"/>
+    </row>
+    <row r="368" spans="1:5">
+      <c r="A368" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B368" s="24"/>
+      <c r="C368" s="24"/>
+      <c r="D368" s="24"/>
+      <c r="E368" s="24"/>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5">
+      <c r="A432" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B432" s="24"/>
+      <c r="C432" s="24"/>
+      <c r="D432" s="24"/>
+      <c r="E432" s="24"/>
+    </row>
+    <row r="433" spans="1:5">
+      <c r="A433" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B433" s="24"/>
+      <c r="C433" s="24"/>
+      <c r="D433" s="24"/>
+      <c r="E433" s="24"/>
+    </row>
+    <row r="434" spans="1:5">
+      <c r="A434" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5">
+      <c r="A486" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B486" s="24"/>
+      <c r="C486" s="24"/>
+      <c r="D486" s="24"/>
+      <c r="E486" s="24"/>
+    </row>
+    <row r="487" spans="1:5">
+      <c r="A487" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B487" s="24"/>
+      <c r="C487" s="24"/>
+      <c r="D487" s="24"/>
+      <c r="E487" s="24"/>
+    </row>
+    <row r="488" spans="1:5">
+      <c r="A488" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:I5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:I5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="5:9">
+      <c r="E2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="5:9">
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="5:9">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="5:9">
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:I5"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>